<commit_message>
Marcado de datos a revisar
</commit_message>
<xml_diff>
--- a/AWS - AZURE.xlsx
+++ b/AWS - AZURE.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samm_\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorodriguez\Desktop\Proyectos\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9EF782-CBA7-465C-B662-4A7BDB24FAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A3FD98DE-3F52-4CD3-859F-C11E884E4417}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="AWS" sheetId="1" r:id="rId1"/>
@@ -463,8 +462,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,8 +518,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,8 +552,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -569,12 +581,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -584,9 +612,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -612,15 +637,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Cálculo" xfId="2" builtinId="22"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -932,304 +964,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354EDEA4-1033-4AE1-BFAF-5DD21646880E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="9" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://aws.amazon.com/ec2/?did=ft_card&amp;trk=ft_card" xr:uid="{02F0C0FD-93B9-45EB-857B-33D972719F52}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://aws.amazon.com/s3/?did=ft_card&amp;trk=ft_card" xr:uid="{03A930B4-0C7B-4040-A27F-E2A63E8E3FC0}"/>
-    <hyperlink ref="C3" r:id="rId3" display="https://aws.amazon.com/rds/?did=ft_card&amp;trk=ft_card" xr:uid="{9A674FF5-9D01-422D-A903-80E812F86E26}"/>
-    <hyperlink ref="D3" r:id="rId4" display="https://aws.amazon.com/dynamodb/?did=ft_card&amp;trk=ft_card" xr:uid="{B8CC289A-818A-40E7-839E-14DB20410563}"/>
-    <hyperlink ref="E3" r:id="rId5" display="https://aws.amazon.com/sagemaker/?did=ft_card&amp;trk=ft_card" xr:uid="{103C6C21-649B-4102-8BE3-535D23D83E5E}"/>
-    <hyperlink ref="F3" r:id="rId6" display="https://aws.amazon.com/lambda/?did=ft_card&amp;trk=ft_card" xr:uid="{262CC590-06D8-4F64-815A-1E933054E6C3}"/>
-    <hyperlink ref="G3" r:id="rId7" display="https://aws.amazon.com/lightsail/?did=ft_card&amp;trk=ft_card" xr:uid="{3B261B84-EA26-4ACA-A216-7C821F5D561A}"/>
-    <hyperlink ref="H3" r:id="rId8" display="https://aws.amazon.com/guardduty/?did=ft_card&amp;trk=ft_card" xr:uid="{7DA637E0-8118-4252-9993-074BAB3ACDFE}"/>
-    <hyperlink ref="I3" r:id="rId9" display="https://aws.amazon.com/sns/?did=ft_card&amp;trk=ft_card" xr:uid="{1A1DA9F0-5A27-4DDB-AC1F-2AA1F74CA013}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FEC20B-6BB7-4272-B8D8-10CE9A5A08A8}">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1240,140 +992,420 @@
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
     </row>
+    <row r="2" spans="1:9" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="143.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="https://aws.amazon.com/ec2/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://aws.amazon.com/s3/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="C3" r:id="rId3" display="https://aws.amazon.com/rds/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://aws.amazon.com/dynamodb/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="E3" r:id="rId5" display="https://aws.amazon.com/sagemaker/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="F3" r:id="rId6" display="https://aws.amazon.com/lambda/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="G3" r:id="rId7" display="https://aws.amazon.com/lightsail/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="H3" r:id="rId8" display="https://aws.amazon.com/guardduty/?did=ft_card&amp;trk=ft_card"/>
+    <hyperlink ref="I3" r:id="rId9" display="https://aws.amazon.com/sns/?did=ft_card&amp;trk=ft_card"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+    </row>
     <row r="2" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="12" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="12" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1382,5 +1414,6 @@
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>